<commit_message>
save bib plus changed figure
</commit_message>
<xml_diff>
--- a/thesis_bibilo_save.xlsx
+++ b/thesis_bibilo_save.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="112">
   <si>
     <t xml:space="preserve">Alexej Abyzov, Shantao Li, Daniel Rhee Kim, Marghoob Mohiyuddin, Adrian M. Sttz, Nicholas F. Parrish, Xinmeng Jasmine Mu, Wyatt Clark, Ken Chen, Matthew Hurles, Jan O. Korbel, Hugo Y. K. Lam, Charles Lee and Mark B. Gerstein
 Analysis of deletion breakpoints from 1,092 humans reveals details of mutation mechanisms Nature CommunicationsBioinformatics published June 1, 2015 </t>
@@ -1014,6 +1014,623 @@
   </si>
   <si>
     <t xml:space="preserve">Griffith, M., Griffith, O. L., Coffman, A. C., Weible, J. V., McMichael, J. F., Spies, N. C., ... &amp; Miller, C. A. (2013). DGIdb: mining the druggable genome. Nature methods, 10(12), 1209-1210.
+Chicago 
+</t>
+  </si>
+  <si>
+    <r>
+      <t>Janitz, M. (Ed.). (2011). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Next-generation genome sequencing: towards personalized medicine</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>. John Wiley &amp; Sons.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Wei, Z., Wang, W., Hu, P., Lyon, G. J., &amp; Hakonarson, H. (2011). SNVer: a statistical tool for variant calling in analysis of pooled or individual next-generation sequencing data. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Nucleic acids research</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>39</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(19), e132-e132.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Lam, H. Y., Clark, M. J., Chen, R., Chen, R., Natsoulis, G., O'huallachain, M., ... &amp; Butte, A. J. (2012). Performance comparison of whole-genome sequencing platforms. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Nature biotechnology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(1), 78-82.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Lusci, A., Pollastri, G., &amp; Baldi, P. (2013). Deep architectures and deep learning in chemoinformatics: the prediction of aqueous solubility for drug-like molecules. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Journal of chemical information and modeling</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>53</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(7), 1563.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Sun, Y., Wang, X., &amp; Tang, X. (2014). Deep learning face representation from predicting 10,000 classes. In </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Proceedings of the IEEE Conference on Computer Vision and Pattern Recognition</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (pp. 1891-1898).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Silver, D., Huang, A., Maddison, C. J., Guez, A., Sifre, L., Van Den Driessche, G., ... &amp; Dieleman, S. (2016). Mastering the game of Go with deep neural networks and tree search. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Nature</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>529</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(7587), 484-489.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Moreau, Y., &amp; Tranchevent, L. C. (2012). Computational tools for prioritizing candidate genes: boosting disease gene discovery. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Nature Reviews Genetics</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>13</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(8), 523-536.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Wang, K., Li, M., &amp; Hakonarson, H. (2010). ANNOVAR: functional annotation of genetic variants from high-throughput sequencing data. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Nucleic acids research</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>38</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(16), e164-e164.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Anthimopoulos, M., Christodoulidis, S., Ebner, L., Christe, A., &amp; Mougiakakou, S. (2016). Lung pattern classification for interstitial lung diseases using a deep convolutional neural network. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>IEEE transactions on medical imaging</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>35</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(5), 1207-1216.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Landrum, M. J., Lee, J. M., Riley, G. R., Jang, W., Rubinstein, W. S., Church, D. M., &amp; Maglott, D. R. (2014). ClinVar: public archive of relationships among sequence variation and human phenotype. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Nucleic acids research</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>42</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(D1), D980-D985.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Schork, N. J., Murray, S. S., Frazer, K. A., &amp; Topol, E. J. (2009). Common vs. rare allele hypotheses for complex diseases. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Current opinion in genetics &amp; development</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>19</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(3), 212-219.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Knudson, A. G. (2001). Two genetic hits (more or less) to cancer. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Nature Reviews Cancer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(2), 157-162.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Alizadeh, A. A., Eisen, M. B., Davis, R. E., Ma, C., Lossos, I. S., Rosenwald, A., ... &amp; Powell, J. I. (2000). Distinct types of diffuse large B-cell lymphoma identified by gene expression profiling. Nature, 403(6769), 503-511.
+Chicago 
+</t>
+  </si>
+  <si>
+    <r>
+      <t>Tentler, J. J., Tan, A. C., Weekes, C. D., Jimeno, A., Leong, S., Pitts, T. M., ... &amp; Eckhardt, S. G. (2012). Patient-derived tumour xenografts as models for oncology drug development. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Nature reviews Clinical oncology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(6), 338-350.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Marron, T. U., Joyce, E. Y., &amp; Cunningham-Rundles, C. (2012). Toll-like receptor function in primary B cell defects. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Frontiers in bioscience (Elite edition)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, 1853.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Kelly, M. G., Alvero, A. B., Chen, R., Silasi, D. A., Abrahams, V. M., Chan, S., ... &amp; Mor, G. (2006). TLR-4 signaling promotes tumor growth and paclitaxel chemoresistance in ovarian cancer. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Cancer research</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>66</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(7), 3859-3868.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Balkwill, F., &amp; Mantovani, A. (2001). Inflammation and cancer: back to Virchow?. The lancet, 357(9255), 539-545.
 Chicago 
 </t>
   </si>
@@ -1171,7 +1788,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1349,6 +1966,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1512,13 +2135,18 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2104,10 +2732,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A61"/>
+  <dimension ref="A1:B78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2193,213 +2821,213 @@
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>51</v>
+      <c r="A21" s="2" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>53</v>
+      <c r="A24" s="2" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>54</v>
+      <c r="A26" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
-        <v>74</v>
+      <c r="A32" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>86</v>
+      <c r="A35" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>60</v>
+      <c r="A36" s="2" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>61</v>
+      <c r="A38" s="2" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
-        <v>79</v>
+      <c r="A39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>63</v>
+      <c r="A42" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>65</v>
+      <c r="A44" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
-        <v>83</v>
+      <c r="A48" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>66</v>
+      <c r="A50" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>35</v>
+      <c r="A51" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>67</v>
+        <v>30</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
-        <v>81</v>
+      <c r="A53" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>68</v>
+      <c r="A54" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>69</v>
+      <c r="A55" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
-        <v>75</v>
+      <c r="A56" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" s="2" t="s">
-        <v>78</v>
+      <c r="A57" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
@@ -2408,18 +3036,106 @@
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" s="2" t="s">
-        <v>93</v>
+      <c r="A60" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" s="3" t="s">
-        <v>94</v>
+      <c r="A61" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B74" s="4"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B75" s="4"/>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B76" s="5"/>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" s="3" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:A58">
-    <sortCondition ref="A58"/>
+  <sortState ref="A2:A67">
+    <sortCondition ref="A67"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Rewrites before grammar changes
</commit_message>
<xml_diff>
--- a/thesis_bibilo_save.xlsx
+++ b/thesis_bibilo_save.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="126">
   <si>
     <t xml:space="preserve">Alexej Abyzov, Shantao Li, Daniel Rhee Kim, Marghoob Mohiyuddin, Adrian M. Sttz, Nicholas F. Parrish, Xinmeng Jasmine Mu, Wyatt Clark, Ken Chen, Matthew Hurles, Jan O. Korbel, Hugo Y. K. Lam, Charles Lee and Mark B. Gerstein
 Analysis of deletion breakpoints from 1,092 humans reveals details of mutation mechanisms Nature CommunicationsBioinformatics published June 1, 2015 </t>
@@ -1633,6 +1633,492 @@
     <t xml:space="preserve">Balkwill, F., &amp; Mantovani, A. (2001). Inflammation and cancer: back to Virchow?. The lancet, 357(9255), 539-545.
 Chicago 
 </t>
+  </si>
+  <si>
+    <r>
+      <t>Zeiler, M. D. (2012). ADADELTA: an adaptive learning rate method. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>arXiv preprint arXiv:1212.5701</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>CLC bio. (2011). Genomics Workbench User Manual 4.8. Finlandsgade 10-12 DK- 8200 Aarhus N, Denmark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sutskever, I., Martens, J., Dahl, G. E., &amp; Hinton, G. E. (2013). On the importance of initialization and momentum in deep learning. ICML (3), 28, 1139-1147.
+Chicago 
+</t>
+  </si>
+  <si>
+    <r>
+      <t>Bengio, Y., Simard, P., &amp; Frasconi, P. (1994). Learning long-term dependencies with gradient descent is difficult. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>IEEE transactions on neural networks</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(2), 157-166.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Chawla, N. V. (2005). Data mining for imbalanced datasets: An overview. In </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Data mining and knowledge discovery handbook</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (pp. 853-867). Springer US.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Lee, I. H., Sohn, M., Lim, H. J., Yoon, S., Oh, H., Shin, S., ... &amp; Noh, D. Y. (2014). Ahnak functions as a tumor suppressor via modulation of TGFβ/Smad signaling pathway. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Oncogene</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>33</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(38), 4675-4684.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Amagai, M. (2004). A mystery of AHNAK/desmoyokin still goes on. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Journal of investigative dermatology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>123</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(4), xiv.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Shtivelman, E., Cohen, F. E., &amp; Bishop, J. M. (1992). A human gene (AHNAK) encoding an unusually large protein with a 1.2-microns polyionic rod structure. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Proceedings of the National Academy of Sciences</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>89</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(12), 5472-5476.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Weniger, M. A., Pulford, K., Gesk, S., Ehrlich, S., Banham, A. H., Lyne, L., ... &amp; Barth, T. F. E. (2006). Gains of the proto-oncogene BCL11A and nuclear accumulation of BCL11AXL protein are frequent in primary mediastinal B-cell lymphoma. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Leukemia</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(10), 1880-1880.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Satterwhite, E., Sonoki, T., Willis, T. G., Harder, L., Nowak, R., Arriola, E. L., ... &amp; Schlegelberger, B. (2001). The BCL11 gene family: involvement of BCL11A in lymphoid malignancies. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Blood</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>98</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(12), 3413-3420.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Zhang, H., Gao, J., Zhao, Z., Li, M., &amp; Liu, C. (2014). Clinical implications of SPRR1A expression in diffuse large B-cell lymphomas: a prospective, observational study. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>BMC cancer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>14</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(1), 333.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Slavotinek, A. M. (2016). The Family of Crumbs Genes and Human Disease. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Molecular Syndromology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(5), 274-281.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Lamont, R. E., Tan, W. H., Innes, A. M., Parboosingh, J. S., Schneidman-Duhovny, D., Rajkovic, A., ... &amp; Gray, K. J. (2016). Expansion of phenotype and genotypic data in CRB2-related syndrome. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>European Journal of Human Genetics</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>24</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(10), 1436-1444.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Emara, M., Turner, A. R., &amp; Allalunis-Turner, J. (2014). Adult, embryonic and fetal hemoglobin are expressed in human glioblastoma cells. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>International journal of oncology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>44</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(2), 514-520.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2732,10 +3218,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B78"/>
+  <dimension ref="A1:B92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3131,6 +3617,76 @@
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>111</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92" s="2" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update software versions, plus grammar edits for introduction
</commit_message>
<xml_diff>
--- a/thesis_bibilo_save.xlsx
+++ b/thesis_bibilo_save.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="129">
   <si>
     <t xml:space="preserve">Alexej Abyzov, Shantao Li, Daniel Rhee Kim, Marghoob Mohiyuddin, Adrian M. Sttz, Nicholas F. Parrish, Xinmeng Jasmine Mu, Wyatt Clark, Ken Chen, Matthew Hurles, Jan O. Korbel, Hugo Y. K. Lam, Charles Lee and Mark B. Gerstein
 Analysis of deletion breakpoints from 1,092 humans reveals details of mutation mechanisms Nature CommunicationsBioinformatics published June 1, 2015 </t>
@@ -2119,6 +2119,76 @@
       </rPr>
       <t>(2), 514-520.</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t>Pedregosa, F., Varoquaux, G., Gramfort, A., Michel, V., Thirion, B., Grisel, O., ... &amp; Vanderplas, J. (2011). Scikit-learn: Machine learning in Python. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Journal of Machine Learning Research</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>12</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Oct), 2825-2830.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Van Rossum, G. (2007, June). Python Programming Language. In </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>USENIX Annual Technical Conference</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (Vol. 41, p. 36).</t>
+    </r>
+  </si>
+  <si>
+    <t>Di Tommaso, P., Chatzou, M., Baraja, P. P., &amp; Notredame, C. (2014). A novel tool for highly scalable computational pipelines.</t>
   </si>
 </sst>
 </file>
@@ -3218,10 +3288,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B92"/>
+  <dimension ref="A1:B95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A92" sqref="A92"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3687,6 +3757,21 @@
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>125</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95" s="2" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Grammar edits, plus changes to ensure figure numbering is correct
</commit_message>
<xml_diff>
--- a/thesis_bibilo_save.xlsx
+++ b/thesis_bibilo_save.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="126">
   <si>
     <t xml:space="preserve">Alexej Abyzov, Shantao Li, Daniel Rhee Kim, Marghoob Mohiyuddin, Adrian M. Sttz, Nicholas F. Parrish, Xinmeng Jasmine Mu, Wyatt Clark, Ken Chen, Matthew Hurles, Jan O. Korbel, Hugo Y. K. Lam, Charles Lee and Mark B. Gerstein
 Analysis of deletion breakpoints from 1,092 humans reveals details of mutation mechanisms Nature CommunicationsBioinformatics published June 1, 2015 </t>
@@ -1662,11 +1662,6 @@
     <t>CLC bio. (2011). Genomics Workbench User Manual 4.8. Finlandsgade 10-12 DK- 8200 Aarhus N, Denmark</t>
   </si>
   <si>
-    <t xml:space="preserve">Sutskever, I., Martens, J., Dahl, G. E., &amp; Hinton, G. E. (2013). On the importance of initialization and momentum in deep learning. ICML (3), 28, 1139-1147.
-Chicago 
-</t>
-  </si>
-  <si>
     <r>
       <t>Bengio, Y., Simard, P., &amp; Frasconi, P. (1994). Learning long-term dependencies with gradient descent is difficult. </t>
     </r>
@@ -1711,30 +1706,6 @@
   </si>
   <si>
     <r>
-      <t>Chawla, N. V. (2005). Data mining for imbalanced datasets: An overview. In </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="8"/>
-        <color rgb="FF222222"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Data mining and knowledge discovery handbook</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF222222"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> (pp. 853-867). Springer US.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>Lee, I. H., Sohn, M., Lim, H. J., Yoon, S., Oh, H., Shin, S., ... &amp; Noh, D. Y. (2014). Ahnak functions as a tumor suppressor via modulation of TGFβ/Smad signaling pathway. </t>
     </r>
     <r>
@@ -1946,49 +1917,6 @@
         <family val="2"/>
       </rPr>
       <t>(12), 3413-3420.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Zhang, H., Gao, J., Zhao, Z., Li, M., &amp; Liu, C. (2014). Clinical implications of SPRR1A expression in diffuse large B-cell lymphomas: a prospective, observational study. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="8"/>
-        <color rgb="FF222222"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>BMC cancer</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF222222"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="8"/>
-        <color rgb="FF222222"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>14</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF222222"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(1), 333.</t>
     </r>
   </si>
   <si>
@@ -3288,10 +3216,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B95"/>
+  <dimension ref="A1:B91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3302,481 +3230,461 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>42</v>
+      <c r="A2" s="6" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>90</v>
+      <c r="A11" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>89</v>
+      <c r="A13" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>94</v>
+      <c r="A17" s="2" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>50</v>
+      <c r="A19" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>95</v>
+      <c r="A20" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>82</v>
+      <c r="A22" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>84</v>
+      <c r="A24" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>52</v>
+      <c r="A25" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>97</v>
+      <c r="A26" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>53</v>
+      <c r="A27" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>16</v>
+      <c r="A28" s="2" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>54</v>
+      <c r="A29" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>56</v>
+      <c r="A31" s="2" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>57</v>
+      <c r="A32" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>98</v>
+      <c r="A33" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>58</v>
+      <c r="A34" s="2" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>59</v>
+      <c r="A35" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>74</v>
+        <v>121</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
-        <v>85</v>
+      <c r="A38" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>23</v>
+      <c r="A39" s="2" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
-        <v>86</v>
+      <c r="A40" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
-        <v>87</v>
+      <c r="A42" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
-        <v>79</v>
+      <c r="A44" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>63</v>
+      <c r="A47" s="2" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>65</v>
+      <c r="A49" s="2" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>31</v>
+      <c r="A53" s="2" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
-        <v>99</v>
+      <c r="A55" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>32</v>
+      <c r="A56" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>35</v>
+      <c r="A58" s="2" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>67</v>
+      <c r="A60" s="2" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" s="2" t="s">
-        <v>96</v>
+      <c r="A61" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A62" s="2" t="s">
-        <v>81</v>
+      <c r="A62" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>69</v>
+      <c r="A64" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="2" t="s">
-        <v>75</v>
+      <c r="A65" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>70</v>
+      <c r="A67" s="2" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" s="2" t="s">
-        <v>104</v>
+      <c r="A71" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" s="2" t="s">
-        <v>105</v>
-      </c>
+      <c r="A72" t="s">
+        <v>31</v>
+      </c>
+      <c r="B72" s="4"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>106</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="B73" s="4"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A74" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="B74" s="4"/>
+      <c r="A74" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B74" s="5"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B75" s="4"/>
+      <c r="A75" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B76" s="5"/>
+      <c r="A76" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" s="3" t="s">
-        <v>111</v>
+      <c r="A78" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>113</v>
+        <v>67</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A81" s="3" t="s">
-        <v>114</v>
+      <c r="A81" s="2" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
-        <v>118</v>
+        <v>81</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A86" s="2" t="s">
-        <v>119</v>
+      <c r="A86" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A87" s="2" t="s">
-        <v>120</v>
+      <c r="A87" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
-        <v>121</v>
+        <v>75</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
-        <v>123</v>
+        <v>78</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A91" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A92" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A93" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A94" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A95" s="2" t="s">
-        <v>128</v>
+      <c r="A91" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:A67">
-    <sortCondition ref="A67"/>
+  <sortState ref="A2:A91">
+    <sortCondition ref="A91"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>